<commit_message>
Atualização de arquivos filtrados
</commit_message>
<xml_diff>
--- a/reports/raw-views/assets/tables/meso.xlsx
+++ b/reports/raw-views/assets/tables/meso.xlsx
@@ -531,10 +531,10 @@
         <v>0.2138821315141114</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5411638409713482</v>
+        <v>0.5271737866561241</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5992386752950133</v>
+        <v>0.5802404724073328</v>
       </c>
     </row>
     <row r="5">
@@ -556,10 +556,10 @@
         <v>0.1301192656101645</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2798875599404728</v>
+        <v>0.2820299692918657</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2993344742346453</v>
+        <v>0.3163706874128024</v>
       </c>
     </row>
     <row r="6">
@@ -581,10 +581,10 @@
         <v>0.1234062892378717</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1222599453834232</v>
+        <v>0.1273308470964305</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1187893397616177</v>
+        <v>0.09794486453172768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>